<commit_message>
modify extension description, add xls file for records example
</commit_message>
<xml_diff>
--- a/Documentation/data_to_be_import_example.xlsx
+++ b/Documentation/data_to_be_import_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF84637-A4B4-495B-86C7-C4447BA4E997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6C154B-56C4-4EF1-879B-D6BC598F90FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="3480" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -135,10 +135,10 @@
     <t>Source host</t>
   </si>
   <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>End date</t>
+    <t>Start date (m/d/y) or (d-m-y)</t>
+  </si>
+  <si>
+    <t>End date (m/d/y) or (d-m-y)</t>
   </si>
 </sst>
 </file>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="5" width="34.140625" customWidth="1"/>
     <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="9" max="9" width="48.42578125" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
@@ -556,7 +556,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G2" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H2">
         <v>307</v>
@@ -582,7 +582,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G3" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H3">
         <v>307</v>
@@ -608,7 +608,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G4" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H4">
         <v>307</v>
@@ -634,7 +634,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G5" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H5">
         <v>307</v>
@@ -660,7 +660,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G6" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H6">
         <v>307</v>
@@ -686,7 +686,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G7" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H7">
         <v>307</v>
@@ -712,7 +712,7 @@
         <v>44540.662499999999</v>
       </c>
       <c r="G8" s="1">
-        <v>44540.662499999999</v>
+        <v>44779.662499999999</v>
       </c>
       <c r="H8">
         <v>307</v>

</xml_diff>

<commit_message>
ignore empty line in the import section, code cleaning, update examples file, update Readme file
</commit_message>
<xml_diff>
--- a/Documentation/data_to_be_import_example.xlsx
+++ b/Documentation/data_to_be_import_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6C154B-56C4-4EF1-879B-D6BC598F90FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4B8D12-C161-4B3E-9F38-E10AF1E80A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="3480" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>true</t>
   </si>
@@ -42,27 +42,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>www.sourceHoste2.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste1.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste3.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste4.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste5.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste6.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste7.com</t>
-  </si>
-  <si>
     <t>/example1</t>
   </si>
   <si>
@@ -84,27 +63,6 @@
     <t>/example7</t>
   </si>
   <si>
-    <t>target1</t>
-  </si>
-  <si>
-    <t>target2</t>
-  </si>
-  <si>
-    <t>target3</t>
-  </si>
-  <si>
-    <t>target4</t>
-  </si>
-  <si>
-    <t>target5</t>
-  </si>
-  <si>
-    <t>target6</t>
-  </si>
-  <si>
-    <t>target7</t>
-  </si>
-  <si>
     <t>title 2</t>
   </si>
   <si>
@@ -132,31 +90,20 @@
     <t>Source path</t>
   </si>
   <si>
-    <t>Source host</t>
-  </si>
-  <si>
-    <t>Start date (m/d/y) or (d-m-y)</t>
-  </si>
-  <si>
-    <t>End date (m/d/y) or (d-m-y)</t>
+    <t>Start date (mm/dd/yyy) or (dd-mm-yyyy)</t>
+  </si>
+  <si>
+    <t>End date (mm/dd/yyy) or (dd-mm-yyyy)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,20 +147,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,245 +445,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="5" width="34.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
-    <col min="9" max="9" width="48.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="48.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E3" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G3" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G2" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H2">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G4" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G5" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G3" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H3">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G6" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G4" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H4">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G7" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G8" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G6" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H6">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G7" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H7">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G8" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H8">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="1"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{BAF4B020-E84C-46DA-B82D-5CE614B262F6}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{60F0DA96-F7D6-4909-85BF-1C383C2D714A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{EC8A0AEB-6AB5-4EE0-8720-CBF656B57A83}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{CA3BFE51-EC8D-43A9-96A0-16F460B962A3}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{195B0EF7-8223-4E51-8475-E6E73E5E04B5}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{B31CDFF5-F514-4E27-B2FC-6DE2AD3E84A6}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{E180B8F8-ECBF-47C4-B622-9E737879BD3C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add csv export for redirections (#8)
Add csv export + minor fixes/text/code refacto
</commit_message>
<xml_diff>
--- a/Documentation/data_to_be_import_example.xlsx
+++ b/Documentation/data_to_be_import_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6C154B-56C4-4EF1-879B-D6BC598F90FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4B8D12-C161-4B3E-9F38-E10AF1E80A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="3480" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>true</t>
   </si>
@@ -42,27 +42,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>www.sourceHoste2.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste1.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste3.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste4.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste5.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste6.com</t>
-  </si>
-  <si>
-    <t>www.sourceHoste7.com</t>
-  </si>
-  <si>
     <t>/example1</t>
   </si>
   <si>
@@ -84,27 +63,6 @@
     <t>/example7</t>
   </si>
   <si>
-    <t>target1</t>
-  </si>
-  <si>
-    <t>target2</t>
-  </si>
-  <si>
-    <t>target3</t>
-  </si>
-  <si>
-    <t>target4</t>
-  </si>
-  <si>
-    <t>target5</t>
-  </si>
-  <si>
-    <t>target6</t>
-  </si>
-  <si>
-    <t>target7</t>
-  </si>
-  <si>
     <t>title 2</t>
   </si>
   <si>
@@ -132,31 +90,20 @@
     <t>Source path</t>
   </si>
   <si>
-    <t>Source host</t>
-  </si>
-  <si>
-    <t>Start date (m/d/y) or (d-m-y)</t>
-  </si>
-  <si>
-    <t>End date (m/d/y) or (d-m-y)</t>
+    <t>Start date (mm/dd/yyy) or (dd-mm-yyyy)</t>
+  </si>
+  <si>
+    <t>End date (mm/dd/yyy) or (dd-mm-yyyy)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,20 +147,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,245 +445,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="5" width="34.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
-    <col min="9" max="9" width="48.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="48.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E3" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G3" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G2" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H2">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G4" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G5" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G3" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H3">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G6" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G4" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H4">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G7" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44905.662499999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45144.662499999999</v>
+      </c>
+      <c r="G8" s="3">
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G6" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H6">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G7" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H7">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1">
-        <v>44540.662499999999</v>
-      </c>
-      <c r="G8" s="1">
-        <v>44779.662499999999</v>
-      </c>
-      <c r="H8">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="1"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{BAF4B020-E84C-46DA-B82D-5CE614B262F6}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{60F0DA96-F7D6-4909-85BF-1C383C2D714A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{EC8A0AEB-6AB5-4EE0-8720-CBF656B57A83}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{CA3BFE51-EC8D-43A9-96A0-16F460B962A3}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{195B0EF7-8223-4E51-8475-E6E73E5E04B5}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{B31CDFF5-F514-4E27-B2FC-6DE2AD3E84A6}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{E180B8F8-ECBF-47C4-B622-9E737879BD3C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>